<commit_message>
add supplemental figures, update maps
</commit_message>
<xml_diff>
--- a/exp_to_figures.xlsx
+++ b/exp_to_figures.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="278">
   <si>
     <t>Raw File</t>
   </si>
@@ -46,13 +46,16 @@
     <t>Figure S4</t>
   </si>
   <si>
+    <t>Figure S5</t>
+  </si>
+  <si>
     <t>Figure S6</t>
   </si>
   <si>
     <t>Figure S7</t>
   </si>
   <si>
-    <t>Figure S8</t>
+    <t>Figure S10</t>
   </si>
   <si>
     <t>180320S_QC_SQC67A1</t>
@@ -965,7 +968,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="42.57"/>
-    <col customWidth="1" min="2" max="14" width="11.43"/>
+    <col customWidth="1" min="2" max="15" width="11.43"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1011,10 +1014,13 @@
       <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" s="4" t="b">
         <v>1</v>
@@ -1053,12 +1059,15 @@
         <v>1</v>
       </c>
       <c r="N2" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O2" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3" s="4" t="b">
         <v>0</v>
@@ -1097,12 +1106,15 @@
         <v>1</v>
       </c>
       <c r="N3" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O3" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" s="4" t="b">
         <v>0</v>
@@ -1141,12 +1153,15 @@
         <v>1</v>
       </c>
       <c r="N4" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O4" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" s="4" t="b">
         <v>0</v>
@@ -1185,12 +1200,15 @@
         <v>1</v>
       </c>
       <c r="N5" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O5" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" s="4" t="b">
         <v>0</v>
@@ -1229,12 +1247,15 @@
         <v>1</v>
       </c>
       <c r="N6" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O6" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" s="4" t="b">
         <v>0</v>
@@ -1273,12 +1294,15 @@
         <v>1</v>
       </c>
       <c r="N7" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O7" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B8" s="4" t="b">
         <v>0</v>
@@ -1317,12 +1341,15 @@
         <v>1</v>
       </c>
       <c r="N8" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O8" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B9" s="4" t="b">
         <v>0</v>
@@ -1361,12 +1388,15 @@
         <v>1</v>
       </c>
       <c r="N9" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O9" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B10" s="4" t="b">
         <v>0</v>
@@ -1405,12 +1435,15 @@
         <v>1</v>
       </c>
       <c r="N10" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O10" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B11" s="4" t="b">
         <v>0</v>
@@ -1449,12 +1482,15 @@
         <v>1</v>
       </c>
       <c r="N11" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O11" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B12" s="4" t="b">
         <v>0</v>
@@ -1493,12 +1529,15 @@
         <v>1</v>
       </c>
       <c r="N12" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O12" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B13" s="4" t="b">
         <v>0</v>
@@ -1537,12 +1576,15 @@
         <v>1</v>
       </c>
       <c r="N13" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O13" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B14" s="4" t="b">
         <v>0</v>
@@ -1581,12 +1623,15 @@
         <v>1</v>
       </c>
       <c r="N14" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O14" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B15" s="4" t="b">
         <v>0</v>
@@ -1625,12 +1670,15 @@
         <v>1</v>
       </c>
       <c r="N15" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O15" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B16" s="4" t="b">
         <v>0</v>
@@ -1669,12 +1717,15 @@
         <v>1</v>
       </c>
       <c r="N16" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O16" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B17" s="4" t="b">
         <v>0</v>
@@ -1713,12 +1764,15 @@
         <v>1</v>
       </c>
       <c r="N17" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O17" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B18" s="4" t="b">
         <v>0</v>
@@ -1757,12 +1811,15 @@
         <v>1</v>
       </c>
       <c r="N18" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O18" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B19" s="4" t="b">
         <v>1</v>
@@ -1801,12 +1858,15 @@
         <v>1</v>
       </c>
       <c r="N19" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O19" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B20" s="4" t="b">
         <v>0</v>
@@ -1845,12 +1905,15 @@
         <v>1</v>
       </c>
       <c r="N20" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O20" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B21" s="4" t="b">
         <v>0</v>
@@ -1889,12 +1952,15 @@
         <v>1</v>
       </c>
       <c r="N21" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O21" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B22" s="4" t="b">
         <v>0</v>
@@ -1933,12 +1999,15 @@
         <v>1</v>
       </c>
       <c r="N22" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O22" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B23" s="4" t="b">
         <v>0</v>
@@ -1977,12 +2046,15 @@
         <v>1</v>
       </c>
       <c r="N23" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O23" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B24" s="4" t="b">
         <v>0</v>
@@ -2021,12 +2093,15 @@
         <v>1</v>
       </c>
       <c r="N24" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O24" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B25" s="4" t="b">
         <v>0</v>
@@ -2065,12 +2140,15 @@
         <v>1</v>
       </c>
       <c r="N25" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O25" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B26" s="4" t="b">
         <v>0</v>
@@ -2109,12 +2187,15 @@
         <v>1</v>
       </c>
       <c r="N26" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O26" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B27" s="4" t="b">
         <v>0</v>
@@ -2153,12 +2234,15 @@
         <v>1</v>
       </c>
       <c r="N27" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O27" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B28" s="4" t="b">
         <v>0</v>
@@ -2197,12 +2281,15 @@
         <v>1</v>
       </c>
       <c r="N28" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O28" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B29" s="4" t="b">
         <v>1</v>
@@ -2241,12 +2328,15 @@
         <v>1</v>
       </c>
       <c r="N29" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O29" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B30" s="4" t="b">
         <v>1</v>
@@ -2285,12 +2375,15 @@
         <v>1</v>
       </c>
       <c r="N30" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O30" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B31" s="4" t="b">
         <v>0</v>
@@ -2329,12 +2422,15 @@
         <v>1</v>
       </c>
       <c r="N31" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O31" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B32" s="4" t="b">
         <v>0</v>
@@ -2373,12 +2469,15 @@
         <v>1</v>
       </c>
       <c r="N32" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O32" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B33" s="4" t="b">
         <v>0</v>
@@ -2417,12 +2516,15 @@
         <v>1</v>
       </c>
       <c r="N33" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O33" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B34" s="4" t="b">
         <v>0</v>
@@ -2461,12 +2563,15 @@
         <v>1</v>
       </c>
       <c r="N34" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O34" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B35" s="4" t="b">
         <v>0</v>
@@ -2505,12 +2610,15 @@
         <v>1</v>
       </c>
       <c r="N35" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O35" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B36" s="4" t="b">
         <v>0</v>
@@ -2549,12 +2657,15 @@
         <v>1</v>
       </c>
       <c r="N36" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O36" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B37" s="4" t="b">
         <v>0</v>
@@ -2593,12 +2704,15 @@
         <v>1</v>
       </c>
       <c r="N37" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O37" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B38" s="4" t="b">
         <v>0</v>
@@ -2637,12 +2751,15 @@
         <v>1</v>
       </c>
       <c r="N38" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O38" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B39" s="4" t="b">
         <v>0</v>
@@ -2681,12 +2798,15 @@
         <v>1</v>
       </c>
       <c r="N39" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O39" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B40" s="4" t="b">
         <v>0</v>
@@ -2725,12 +2845,15 @@
         <v>1</v>
       </c>
       <c r="N40" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O40" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B41" s="4" t="b">
         <v>0</v>
@@ -2769,12 +2892,15 @@
         <v>1</v>
       </c>
       <c r="N41" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O41" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B42" s="4" t="b">
         <v>0</v>
@@ -2813,12 +2939,15 @@
         <v>1</v>
       </c>
       <c r="N42" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O42" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B43" s="4" t="b">
         <v>0</v>
@@ -2857,12 +2986,15 @@
         <v>1</v>
       </c>
       <c r="N43" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O43" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B44" s="4" t="b">
         <v>0</v>
@@ -2901,12 +3033,15 @@
         <v>1</v>
       </c>
       <c r="N44" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O44" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B45" s="4" t="b">
         <v>0</v>
@@ -2945,12 +3080,15 @@
         <v>1</v>
       </c>
       <c r="N45" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O45" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B46" s="4" t="b">
         <v>0</v>
@@ -2989,12 +3127,15 @@
         <v>1</v>
       </c>
       <c r="N46" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O46" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B47" s="4" t="b">
         <v>0</v>
@@ -3033,12 +3174,15 @@
         <v>1</v>
       </c>
       <c r="N47" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O47" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B48" s="4" t="b">
         <v>0</v>
@@ -3077,12 +3221,15 @@
         <v>1</v>
       </c>
       <c r="N48" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O48" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B49" s="4" t="b">
         <v>1</v>
@@ -3121,12 +3268,15 @@
         <v>1</v>
       </c>
       <c r="N49" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O49" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B50" s="4" t="b">
         <v>1</v>
@@ -3165,12 +3315,15 @@
         <v>1</v>
       </c>
       <c r="N50" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O50" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B51" s="4" t="b">
         <v>0</v>
@@ -3209,12 +3362,15 @@
         <v>1</v>
       </c>
       <c r="N51" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O51" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B52" s="4" t="b">
         <v>0</v>
@@ -3253,12 +3409,15 @@
         <v>1</v>
       </c>
       <c r="N52" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O52" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B53" s="4" t="b">
         <v>0</v>
@@ -3297,12 +3456,15 @@
         <v>1</v>
       </c>
       <c r="N53" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O53" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B54" s="4" t="b">
         <v>0</v>
@@ -3341,12 +3503,15 @@
         <v>1</v>
       </c>
       <c r="N54" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O54" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B55" s="4" t="b">
         <v>0</v>
@@ -3385,12 +3550,15 @@
         <v>1</v>
       </c>
       <c r="N55" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O55" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B56" s="4" t="b">
         <v>1</v>
@@ -3429,12 +3597,15 @@
         <v>1</v>
       </c>
       <c r="N56" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O56" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B57" s="4" t="b">
         <v>1</v>
@@ -3473,12 +3644,15 @@
         <v>1</v>
       </c>
       <c r="N57" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O57" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B58" s="4" t="b">
         <v>0</v>
@@ -3517,12 +3691,15 @@
         <v>1</v>
       </c>
       <c r="N58" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O58" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B59" s="4" t="b">
         <v>0</v>
@@ -3561,12 +3738,15 @@
         <v>1</v>
       </c>
       <c r="N59" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O59" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B60" s="4" t="b">
         <v>0</v>
@@ -3605,12 +3785,15 @@
         <v>1</v>
       </c>
       <c r="N60" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O60" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B61" s="4" t="b">
         <v>1</v>
@@ -3649,12 +3832,15 @@
         <v>1</v>
       </c>
       <c r="N61" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O61" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B62" s="4" t="b">
         <v>1</v>
@@ -3693,12 +3879,15 @@
         <v>1</v>
       </c>
       <c r="N62" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O62" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B63" s="4" t="b">
         <v>0</v>
@@ -3737,12 +3926,15 @@
         <v>1</v>
       </c>
       <c r="N63" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O63" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B64" s="4" t="b">
         <v>0</v>
@@ -3781,12 +3973,15 @@
         <v>1</v>
       </c>
       <c r="N64" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O64" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B65" s="4" t="b">
         <v>0</v>
@@ -3825,12 +4020,15 @@
         <v>1</v>
       </c>
       <c r="N65" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O65" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B66" s="4" t="b">
         <v>0</v>
@@ -3869,12 +4067,15 @@
         <v>1</v>
       </c>
       <c r="N66" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O66" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B67" s="4" t="b">
         <v>1</v>
@@ -3913,12 +4114,15 @@
         <v>1</v>
       </c>
       <c r="N67" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O67" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B68" s="4" t="b">
         <v>0</v>
@@ -3957,12 +4161,15 @@
         <v>1</v>
       </c>
       <c r="N68" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O68" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B69" s="4" t="b">
         <v>0</v>
@@ -4001,12 +4208,15 @@
         <v>1</v>
       </c>
       <c r="N69" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O69" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B70" s="4" t="b">
         <v>0</v>
@@ -4045,12 +4255,15 @@
         <v>1</v>
       </c>
       <c r="N70" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O70" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B71" s="4" t="b">
         <v>1</v>
@@ -4089,12 +4302,15 @@
         <v>1</v>
       </c>
       <c r="N71" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O71" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B72" s="4" t="b">
         <v>0</v>
@@ -4133,12 +4349,15 @@
         <v>1</v>
       </c>
       <c r="N72" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O72" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B73" s="4" t="b">
         <v>0</v>
@@ -4177,12 +4396,15 @@
         <v>1</v>
       </c>
       <c r="N73" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O73" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B74" s="4" t="b">
         <v>0</v>
@@ -4221,12 +4443,15 @@
         <v>1</v>
       </c>
       <c r="N74" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O74" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B75" s="4" t="b">
         <v>0</v>
@@ -4265,12 +4490,15 @@
         <v>1</v>
       </c>
       <c r="N75" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O75" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B76" s="4" t="b">
         <v>0</v>
@@ -4309,12 +4537,15 @@
         <v>1</v>
       </c>
       <c r="N76" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O76" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B77" s="4" t="b">
         <v>0</v>
@@ -4353,12 +4584,15 @@
         <v>1</v>
       </c>
       <c r="N77" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O77" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B78" s="4" t="b">
         <v>0</v>
@@ -4397,12 +4631,15 @@
         <v>1</v>
       </c>
       <c r="N78" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O78" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B79" s="4" t="b">
         <v>0</v>
@@ -4441,12 +4678,15 @@
         <v>1</v>
       </c>
       <c r="N79" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O79" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B80" s="4" t="b">
         <v>0</v>
@@ -4485,12 +4725,15 @@
         <v>1</v>
       </c>
       <c r="N80" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O80" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B81" s="4" t="b">
         <v>0</v>
@@ -4529,12 +4772,15 @@
         <v>1</v>
       </c>
       <c r="N81" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O81" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B82" s="4" t="b">
         <v>0</v>
@@ -4573,12 +4819,15 @@
         <v>1</v>
       </c>
       <c r="N82" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O82" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B83" s="4" t="b">
         <v>0</v>
@@ -4617,12 +4866,15 @@
         <v>1</v>
       </c>
       <c r="N83" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O83" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B84" s="4" t="b">
         <v>0</v>
@@ -4661,12 +4913,15 @@
         <v>1</v>
       </c>
       <c r="N84" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O84" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B85" s="4" t="b">
         <v>0</v>
@@ -4705,12 +4960,15 @@
         <v>1</v>
       </c>
       <c r="N85" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O85" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B86" s="4" t="b">
         <v>0</v>
@@ -4749,12 +5007,15 @@
         <v>1</v>
       </c>
       <c r="N86" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O86" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B87" s="4" t="b">
         <v>0</v>
@@ -4793,12 +5054,15 @@
         <v>1</v>
       </c>
       <c r="N87" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O87" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B88" s="4" t="b">
         <v>0</v>
@@ -4837,12 +5101,15 @@
         <v>1</v>
       </c>
       <c r="N88" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O88" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B89" s="4" t="b">
         <v>0</v>
@@ -4881,12 +5148,15 @@
         <v>1</v>
       </c>
       <c r="N89" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O89" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B90" s="4" t="b">
         <v>0</v>
@@ -4925,12 +5195,15 @@
         <v>1</v>
       </c>
       <c r="N90" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O90" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B91" s="4" t="b">
         <v>0</v>
@@ -4969,12 +5242,15 @@
         <v>1</v>
       </c>
       <c r="N91" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O91" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B92" s="4" t="b">
         <v>0</v>
@@ -5013,12 +5289,15 @@
         <v>1</v>
       </c>
       <c r="N92" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O92" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B93" s="4" t="b">
         <v>0</v>
@@ -5057,12 +5336,15 @@
         <v>1</v>
       </c>
       <c r="N93" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O93" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B94" s="4" t="b">
         <v>0</v>
@@ -5101,12 +5383,15 @@
         <v>1</v>
       </c>
       <c r="N94" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O94" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B95" s="4" t="b">
         <v>1</v>
@@ -5145,12 +5430,15 @@
         <v>1</v>
       </c>
       <c r="N95" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O95" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B96" s="4" t="b">
         <v>1</v>
@@ -5189,12 +5477,15 @@
         <v>1</v>
       </c>
       <c r="N96" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O96" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B97" s="4" t="b">
         <v>0</v>
@@ -5233,12 +5524,15 @@
         <v>1</v>
       </c>
       <c r="N97" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O97" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B98" s="4" t="b">
         <v>0</v>
@@ -5277,12 +5571,15 @@
         <v>1</v>
       </c>
       <c r="N98" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O98" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B99" s="4" t="b">
         <v>1</v>
@@ -5321,12 +5618,15 @@
         <v>1</v>
       </c>
       <c r="N99" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O99" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B100" s="4" t="b">
         <v>1</v>
@@ -5365,12 +5665,15 @@
         <v>1</v>
       </c>
       <c r="N100" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O100" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B101" s="4" t="b">
         <v>0</v>
@@ -5409,12 +5712,15 @@
         <v>1</v>
       </c>
       <c r="N101" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O101" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B102" s="4" t="b">
         <v>0</v>
@@ -5453,12 +5759,15 @@
         <v>1</v>
       </c>
       <c r="N102" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O102" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B103" s="4" t="b">
         <v>0</v>
@@ -5497,12 +5806,15 @@
         <v>1</v>
       </c>
       <c r="N103" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O103" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B104" s="4" t="b">
         <v>0</v>
@@ -5541,12 +5853,15 @@
         <v>1</v>
       </c>
       <c r="N104" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O104" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B105" s="4" t="b">
         <v>0</v>
@@ -5585,12 +5900,15 @@
         <v>1</v>
       </c>
       <c r="N105" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O105" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B106" s="4" t="b">
         <v>0</v>
@@ -5629,12 +5947,15 @@
         <v>1</v>
       </c>
       <c r="N106" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O106" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B107" s="4" t="b">
         <v>0</v>
@@ -5673,12 +5994,15 @@
         <v>1</v>
       </c>
       <c r="N107" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O107" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B108" s="4" t="b">
         <v>0</v>
@@ -5717,12 +6041,15 @@
         <v>1</v>
       </c>
       <c r="N108" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O108" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B109" s="4" t="b">
         <v>0</v>
@@ -5761,12 +6088,15 @@
         <v>1</v>
       </c>
       <c r="N109" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O109" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B110" s="4" t="b">
         <v>0</v>
@@ -5805,12 +6135,15 @@
         <v>1</v>
       </c>
       <c r="N110" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O110" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B111" s="4" t="b">
         <v>0</v>
@@ -5849,12 +6182,15 @@
         <v>1</v>
       </c>
       <c r="N111" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O111" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B112" s="4" t="b">
         <v>0</v>
@@ -5893,12 +6229,15 @@
         <v>1</v>
       </c>
       <c r="N112" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O112" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B113" s="4" t="b">
         <v>0</v>
@@ -5937,12 +6276,15 @@
         <v>1</v>
       </c>
       <c r="N113" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O113" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B114" s="4" t="b">
         <v>1</v>
@@ -5981,12 +6323,15 @@
         <v>1</v>
       </c>
       <c r="N114" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O114" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B115" s="4" t="b">
         <v>1</v>
@@ -6025,12 +6370,15 @@
         <v>1</v>
       </c>
       <c r="N115" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O115" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B116" s="4" t="b">
         <v>1</v>
@@ -6069,12 +6417,15 @@
         <v>1</v>
       </c>
       <c r="N116" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O116" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B117" s="4" t="b">
         <v>1</v>
@@ -6113,12 +6464,15 @@
         <v>1</v>
       </c>
       <c r="N117" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O117" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B118" s="4" t="b">
         <v>0</v>
@@ -6157,12 +6511,15 @@
         <v>1</v>
       </c>
       <c r="N118" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O118" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B119" s="4" t="b">
         <v>0</v>
@@ -6201,12 +6558,15 @@
         <v>1</v>
       </c>
       <c r="N119" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O119" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B120" s="4" t="b">
         <v>0</v>
@@ -6245,12 +6605,15 @@
         <v>1</v>
       </c>
       <c r="N120" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O120" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B121" s="4" t="b">
         <v>0</v>
@@ -6289,12 +6652,15 @@
         <v>1</v>
       </c>
       <c r="N121" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O121" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B122" s="4" t="b">
         <v>0</v>
@@ -6333,12 +6699,15 @@
         <v>1</v>
       </c>
       <c r="N122" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O122" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B123" s="4" t="b">
         <v>1</v>
@@ -6377,12 +6746,15 @@
         <v>1</v>
       </c>
       <c r="N123" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O123" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="5" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B124" s="4" t="b">
         <v>0</v>
@@ -6421,12 +6793,15 @@
         <v>1</v>
       </c>
       <c r="N124" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O124" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B125" s="4" t="b">
         <v>1</v>
@@ -6465,12 +6840,15 @@
         <v>1</v>
       </c>
       <c r="N125" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O125" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B126" s="4" t="b">
         <v>0</v>
@@ -6509,12 +6887,15 @@
         <v>1</v>
       </c>
       <c r="N126" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O126" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B127" s="4" t="b">
         <v>0</v>
@@ -6553,12 +6934,15 @@
         <v>1</v>
       </c>
       <c r="N127" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O127" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B128" s="4" t="b">
         <v>0</v>
@@ -6597,12 +6981,15 @@
         <v>1</v>
       </c>
       <c r="N128" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O128" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B129" s="4" t="b">
         <v>0</v>
@@ -6641,12 +7028,15 @@
         <v>1</v>
       </c>
       <c r="N129" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O129" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B130" s="4" t="b">
         <v>0</v>
@@ -6685,12 +7075,15 @@
         <v>1</v>
       </c>
       <c r="N130" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O130" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B131" s="4" t="b">
         <v>0</v>
@@ -6729,12 +7122,15 @@
         <v>1</v>
       </c>
       <c r="N131" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O131" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B132" s="4" t="b">
         <v>0</v>
@@ -6773,12 +7169,15 @@
         <v>1</v>
       </c>
       <c r="N132" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O132" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B133" s="4" t="b">
         <v>0</v>
@@ -6817,12 +7216,15 @@
         <v>1</v>
       </c>
       <c r="N133" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O133" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B134" s="4" t="b">
         <v>0</v>
@@ -6861,12 +7263,15 @@
         <v>1</v>
       </c>
       <c r="N134" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O134" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B135" s="4" t="b">
         <v>0</v>
@@ -6905,12 +7310,15 @@
         <v>1</v>
       </c>
       <c r="N135" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O135" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B136" s="4" t="b">
         <v>0</v>
@@ -6949,12 +7357,15 @@
         <v>1</v>
       </c>
       <c r="N136" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O136" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B137" s="4" t="b">
         <v>1</v>
@@ -6993,12 +7404,15 @@
         <v>1</v>
       </c>
       <c r="N137" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O137" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B138" s="4" t="b">
         <v>1</v>
@@ -7037,12 +7451,15 @@
         <v>1</v>
       </c>
       <c r="N138" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O138" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B139" s="4" t="b">
         <v>1</v>
@@ -7081,12 +7498,15 @@
         <v>1</v>
       </c>
       <c r="N139" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O139" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B140" s="4" t="b">
         <v>1</v>
@@ -7125,12 +7545,15 @@
         <v>1</v>
       </c>
       <c r="N140" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O140" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B141" s="4" t="b">
         <v>0</v>
@@ -7169,12 +7592,15 @@
         <v>1</v>
       </c>
       <c r="N141" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O141" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B142" s="4" t="b">
         <v>0</v>
@@ -7213,12 +7639,15 @@
         <v>1</v>
       </c>
       <c r="N142" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O142" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B143" s="4" t="b">
         <v>0</v>
@@ -7257,12 +7686,15 @@
         <v>1</v>
       </c>
       <c r="N143" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O143" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B144" s="4" t="b">
         <v>0</v>
@@ -7301,12 +7733,15 @@
         <v>1</v>
       </c>
       <c r="N144" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O144" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="5" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B145" s="4" t="b">
         <v>1</v>
@@ -7345,12 +7780,15 @@
         <v>1</v>
       </c>
       <c r="N145" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O145" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B146" s="4" t="b">
         <v>0</v>
@@ -7389,12 +7827,15 @@
         <v>1</v>
       </c>
       <c r="N146" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O146" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B147" s="4" t="b">
         <v>0</v>
@@ -7433,12 +7874,15 @@
         <v>1</v>
       </c>
       <c r="N147" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O147" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="5" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B148" s="4" t="b">
         <v>1</v>
@@ -7477,12 +7921,15 @@
         <v>1</v>
       </c>
       <c r="N148" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O148" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B149" s="4" t="b">
         <v>0</v>
@@ -7521,12 +7968,15 @@
         <v>1</v>
       </c>
       <c r="N149" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O149" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B150" s="4" t="b">
         <v>0</v>
@@ -7565,12 +8015,15 @@
         <v>1</v>
       </c>
       <c r="N150" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O150" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B151" s="4" t="b">
         <v>0</v>
@@ -7609,12 +8062,15 @@
         <v>1</v>
       </c>
       <c r="N151" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O151" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B152" s="4" t="b">
         <v>0</v>
@@ -7653,12 +8109,15 @@
         <v>1</v>
       </c>
       <c r="N152" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O152" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B153" s="4" t="b">
         <v>0</v>
@@ -7697,12 +8156,15 @@
         <v>1</v>
       </c>
       <c r="N153" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O153" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="5" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B154" s="4" t="b">
         <v>1</v>
@@ -7741,12 +8203,15 @@
         <v>1</v>
       </c>
       <c r="N154" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O154" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="5" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B155" s="4" t="b">
         <v>0</v>
@@ -7785,12 +8250,15 @@
         <v>1</v>
       </c>
       <c r="N155" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O155" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="5" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B156" s="4" t="b">
         <v>0</v>
@@ -7829,12 +8297,15 @@
         <v>1</v>
       </c>
       <c r="N156" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O156" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B157" s="4" t="b">
         <v>0</v>
@@ -7873,12 +8344,15 @@
         <v>1</v>
       </c>
       <c r="N157" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O157" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B158" s="4" t="b">
         <v>0</v>
@@ -7917,12 +8391,15 @@
         <v>1</v>
       </c>
       <c r="N158" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O158" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="5" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B159" s="4" t="b">
         <v>0</v>
@@ -7961,12 +8438,15 @@
         <v>1</v>
       </c>
       <c r="N159" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O159" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B160" s="4" t="b">
         <v>1</v>
@@ -8005,12 +8485,15 @@
         <v>1</v>
       </c>
       <c r="N160" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O160" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B161" s="4" t="b">
         <v>1</v>
@@ -8049,12 +8532,15 @@
         <v>1</v>
       </c>
       <c r="N161" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O161" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B162" s="4" t="b">
         <v>0</v>
@@ -8093,12 +8579,15 @@
         <v>1</v>
       </c>
       <c r="N162" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O162" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="5" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B163" s="4" t="b">
         <v>1</v>
@@ -8137,12 +8626,15 @@
         <v>1</v>
       </c>
       <c r="N163" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O163" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="5" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B164" s="4" t="b">
         <v>0</v>
@@ -8181,12 +8673,15 @@
         <v>1</v>
       </c>
       <c r="N164" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O164" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B165" s="4" t="b">
         <v>1</v>
@@ -8225,12 +8720,15 @@
         <v>1</v>
       </c>
       <c r="N165" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O165" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B166" s="4" t="b">
         <v>0</v>
@@ -8269,12 +8767,15 @@
         <v>1</v>
       </c>
       <c r="N166" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O166" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B167" s="4" t="b">
         <v>1</v>
@@ -8313,12 +8814,15 @@
         <v>1</v>
       </c>
       <c r="N167" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O167" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B168" s="4" t="b">
         <v>0</v>
@@ -8357,12 +8861,15 @@
         <v>1</v>
       </c>
       <c r="N168" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O168" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B169" s="4" t="b">
         <v>1</v>
@@ -8401,12 +8908,15 @@
         <v>1</v>
       </c>
       <c r="N169" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O169" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="5" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B170" s="4" t="b">
         <v>0</v>
@@ -8445,12 +8955,15 @@
         <v>1</v>
       </c>
       <c r="N170" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O170" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="5" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B171" s="4" t="b">
         <v>1</v>
@@ -8489,12 +9002,15 @@
         <v>1</v>
       </c>
       <c r="N171" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O171" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B172" s="4" t="b">
         <v>0</v>
@@ -8533,12 +9049,15 @@
         <v>1</v>
       </c>
       <c r="N172" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O172" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="5" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B173" s="4" t="b">
         <v>1</v>
@@ -8577,12 +9096,15 @@
         <v>1</v>
       </c>
       <c r="N173" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O173" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="5" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B174" s="4" t="b">
         <v>0</v>
@@ -8621,12 +9143,15 @@
         <v>1</v>
       </c>
       <c r="N174" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O174" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B175" s="4" t="b">
         <v>0</v>
@@ -8665,12 +9190,15 @@
         <v>1</v>
       </c>
       <c r="N175" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O175" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="5" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B176" s="4" t="b">
         <v>0</v>
@@ -8709,12 +9237,15 @@
         <v>1</v>
       </c>
       <c r="N176" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O176" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B177" s="4" t="b">
         <v>0</v>
@@ -8753,12 +9284,15 @@
         <v>1</v>
       </c>
       <c r="N177" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O177" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B178" s="4" t="b">
         <v>0</v>
@@ -8797,12 +9331,15 @@
         <v>1</v>
       </c>
       <c r="N178" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O178" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="5" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B179" s="4" t="b">
         <v>0</v>
@@ -8841,12 +9378,15 @@
         <v>1</v>
       </c>
       <c r="N179" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O179" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B180" s="4" t="b">
         <v>0</v>
@@ -8885,12 +9425,15 @@
         <v>1</v>
       </c>
       <c r="N180" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O180" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="5" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B181" s="4" t="b">
         <v>1</v>
@@ -8929,12 +9472,15 @@
         <v>1</v>
       </c>
       <c r="N181" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O181" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="5" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B182" s="4" t="b">
         <v>1</v>
@@ -8973,12 +9519,15 @@
         <v>1</v>
       </c>
       <c r="N182" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O182" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B183" s="4" t="b">
         <v>1</v>
@@ -9017,12 +9566,15 @@
         <v>1</v>
       </c>
       <c r="N183" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O183" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B184" s="4" t="b">
         <v>0</v>
@@ -9061,12 +9613,15 @@
         <v>1</v>
       </c>
       <c r="N184" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O184" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="5" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B185" s="4" t="b">
         <v>1</v>
@@ -9105,12 +9660,15 @@
         <v>1</v>
       </c>
       <c r="N185" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O185" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="5" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B186" s="4" t="b">
         <v>1</v>
@@ -9149,12 +9707,15 @@
         <v>1</v>
       </c>
       <c r="N186" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O186" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="5" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B187" s="4" t="b">
         <v>0</v>
@@ -9193,12 +9754,15 @@
         <v>1</v>
       </c>
       <c r="N187" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O187" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="5" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B188" s="4" t="b">
         <v>0</v>
@@ -9237,12 +9801,15 @@
         <v>1</v>
       </c>
       <c r="N188" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O188" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="5" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B189" s="4" t="b">
         <v>1</v>
@@ -9281,12 +9848,15 @@
         <v>1</v>
       </c>
       <c r="N189" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O189" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="5" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B190" s="4" t="b">
         <v>0</v>
@@ -9325,12 +9895,15 @@
         <v>1</v>
       </c>
       <c r="N190" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O190" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B191" s="4" t="b">
         <v>0</v>
@@ -9369,12 +9942,15 @@
         <v>1</v>
       </c>
       <c r="N191" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O191" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="5" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B192" s="4" t="b">
         <v>1</v>
@@ -9413,12 +9989,15 @@
         <v>1</v>
       </c>
       <c r="N192" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O192" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="5" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B193" s="4" t="b">
         <v>1</v>
@@ -9457,12 +10036,15 @@
         <v>1</v>
       </c>
       <c r="N193" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O193" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="5" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B194" s="4" t="b">
         <v>0</v>
@@ -9501,12 +10083,15 @@
         <v>1</v>
       </c>
       <c r="N194" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O194" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B195" s="4" t="b">
         <v>0</v>
@@ -9545,12 +10130,15 @@
         <v>1</v>
       </c>
       <c r="N195" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O195" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="5" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B196" s="4" t="b">
         <v>0</v>
@@ -9589,12 +10177,15 @@
         <v>1</v>
       </c>
       <c r="N196" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O196" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B197" s="4" t="b">
         <v>0</v>
@@ -9633,12 +10224,15 @@
         <v>1</v>
       </c>
       <c r="N197" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O197" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="5" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B198" s="4" t="b">
         <v>0</v>
@@ -9677,12 +10271,15 @@
         <v>1</v>
       </c>
       <c r="N198" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O198" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="5" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B199" s="4" t="b">
         <v>0</v>
@@ -9721,12 +10318,15 @@
         <v>1</v>
       </c>
       <c r="N199" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O199" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="5" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B200" s="4" t="b">
         <v>0</v>
@@ -9765,12 +10365,15 @@
         <v>1</v>
       </c>
       <c r="N200" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O200" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B201" s="4" t="b">
         <v>0</v>
@@ -9809,12 +10412,15 @@
         <v>1</v>
       </c>
       <c r="N201" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O201" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B202" s="4" t="b">
         <v>0</v>
@@ -9853,12 +10459,15 @@
         <v>1</v>
       </c>
       <c r="N202" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O202" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="5" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B203" s="4" t="b">
         <v>0</v>
@@ -9897,12 +10506,15 @@
         <v>1</v>
       </c>
       <c r="N203" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O203" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B204" s="4" t="b">
         <v>0</v>
@@ -9941,12 +10553,15 @@
         <v>1</v>
       </c>
       <c r="N204" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O204" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B205" s="4" t="b">
         <v>0</v>
@@ -9985,12 +10600,15 @@
         <v>1</v>
       </c>
       <c r="N205" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O205" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="5" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B206" s="4" t="b">
         <v>0</v>
@@ -10029,12 +10647,15 @@
         <v>1</v>
       </c>
       <c r="N206" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O206" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="5" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B207" s="4" t="b">
         <v>0</v>
@@ -10073,12 +10694,15 @@
         <v>1</v>
       </c>
       <c r="N207" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O207" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="5" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B208" s="4" t="b">
         <v>0</v>
@@ -10117,12 +10741,15 @@
         <v>1</v>
       </c>
       <c r="N208" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O208" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="5" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B209" s="4" t="b">
         <v>0</v>
@@ -10161,12 +10788,15 @@
         <v>1</v>
       </c>
       <c r="N209" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O209" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="5" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B210" s="4" t="b">
         <v>0</v>
@@ -10205,12 +10835,15 @@
         <v>1</v>
       </c>
       <c r="N210" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O210" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="5" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B211" s="4" t="b">
         <v>0</v>
@@ -10249,12 +10882,15 @@
         <v>1</v>
       </c>
       <c r="N211" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O211" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="5" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B212" s="4" t="b">
         <v>0</v>
@@ -10293,12 +10929,15 @@
         <v>1</v>
       </c>
       <c r="N212" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O212" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="5" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B213" s="4" t="b">
         <v>0</v>
@@ -10337,12 +10976,15 @@
         <v>1</v>
       </c>
       <c r="N213" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O213" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="5" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B214" s="4" t="b">
         <v>0</v>
@@ -10381,12 +11023,15 @@
         <v>1</v>
       </c>
       <c r="N214" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O214" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="5" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B215" s="4" t="b">
         <v>0</v>
@@ -10425,12 +11070,15 @@
         <v>1</v>
       </c>
       <c r="N215" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O215" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="5" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B216" s="4" t="b">
         <v>0</v>
@@ -10469,12 +11117,15 @@
         <v>1</v>
       </c>
       <c r="N216" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O216" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="5" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B217" s="4" t="b">
         <v>0</v>
@@ -10513,12 +11164,15 @@
         <v>1</v>
       </c>
       <c r="N217" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O217" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="5" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B218" s="4" t="b">
         <v>0</v>
@@ -10557,12 +11211,15 @@
         <v>1</v>
       </c>
       <c r="N218" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O218" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="5" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B219" s="4" t="b">
         <v>0</v>
@@ -10601,12 +11258,15 @@
         <v>1</v>
       </c>
       <c r="N219" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O219" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="5" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B220" s="4" t="b">
         <v>0</v>
@@ -10645,12 +11305,15 @@
         <v>1</v>
       </c>
       <c r="N220" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O220" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="5" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B221" s="4" t="b">
         <v>0</v>
@@ -10689,12 +11352,15 @@
         <v>1</v>
       </c>
       <c r="N221" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O221" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="5" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B222" s="4" t="b">
         <v>0</v>
@@ -10733,12 +11399,15 @@
         <v>1</v>
       </c>
       <c r="N222" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O222" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="5" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B223" s="4" t="b">
         <v>0</v>
@@ -10777,12 +11446,15 @@
         <v>1</v>
       </c>
       <c r="N223" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O223" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="5" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B224" s="4" t="b">
         <v>0</v>
@@ -10821,12 +11493,15 @@
         <v>1</v>
       </c>
       <c r="N224" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O224" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="5" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B225" s="4" t="b">
         <v>0</v>
@@ -10865,12 +11540,15 @@
         <v>1</v>
       </c>
       <c r="N225" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O225" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="5" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B226" s="4" t="b">
         <v>0</v>
@@ -10909,12 +11587,15 @@
         <v>1</v>
       </c>
       <c r="N226" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O226" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="5" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B227" s="4" t="b">
         <v>0</v>
@@ -10953,12 +11634,15 @@
         <v>1</v>
       </c>
       <c r="N227" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O227" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="5" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B228" s="4" t="b">
         <v>0</v>
@@ -10997,12 +11681,15 @@
         <v>1</v>
       </c>
       <c r="N228" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O228" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="5" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B229" s="4" t="b">
         <v>0</v>
@@ -11041,12 +11728,15 @@
         <v>1</v>
       </c>
       <c r="N229" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O229" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="5" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B230" s="4" t="b">
         <v>0</v>
@@ -11085,12 +11775,15 @@
         <v>1</v>
       </c>
       <c r="N230" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O230" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="5" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B231" s="4" t="b">
         <v>0</v>
@@ -11129,12 +11822,15 @@
         <v>1</v>
       </c>
       <c r="N231" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O231" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="5" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B232" s="4" t="b">
         <v>0</v>
@@ -11173,12 +11869,15 @@
         <v>1</v>
       </c>
       <c r="N232" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O232" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="5" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B233" s="4" t="b">
         <v>0</v>
@@ -11217,12 +11916,15 @@
         <v>1</v>
       </c>
       <c r="N233" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O233" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="5" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B234" s="4" t="b">
         <v>0</v>
@@ -11261,12 +11963,15 @@
         <v>1</v>
       </c>
       <c r="N234" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O234" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="5" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B235" s="4" t="b">
         <v>0</v>
@@ -11305,12 +12010,15 @@
         <v>1</v>
       </c>
       <c r="N235" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O235" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="8" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B236" s="4" t="b">
         <v>0</v>
@@ -11349,12 +12057,15 @@
         <v>1</v>
       </c>
       <c r="N236" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O236" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="8" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B237" s="4" t="b">
         <v>0</v>
@@ -11393,12 +12104,15 @@
         <v>1</v>
       </c>
       <c r="N237" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O237" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="8" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B238" s="4" t="b">
         <v>0</v>
@@ -11437,12 +12151,15 @@
         <v>1</v>
       </c>
       <c r="N238" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O238" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="8" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B239" s="4" t="b">
         <v>0</v>
@@ -11481,12 +12198,15 @@
         <v>1</v>
       </c>
       <c r="N239" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O239" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="8" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B240" s="4" t="b">
         <v>0</v>
@@ -11525,12 +12245,15 @@
         <v>1</v>
       </c>
       <c r="N240" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O240" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="8" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B241" s="4" t="b">
         <v>0</v>
@@ -11569,12 +12292,15 @@
         <v>1</v>
       </c>
       <c r="N241" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O241" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="8" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B242" s="4" t="b">
         <v>0</v>
@@ -11613,12 +12339,15 @@
         <v>1</v>
       </c>
       <c r="N242" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O242" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="8" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B243" s="4" t="b">
         <v>0</v>
@@ -11657,12 +12386,15 @@
         <v>1</v>
       </c>
       <c r="N243" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O243" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="6" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B244" s="4" t="b">
         <v>0</v>
@@ -11701,12 +12433,15 @@
         <v>1</v>
       </c>
       <c r="N244" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O244" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="8" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B245" s="4" t="b">
         <v>0</v>
@@ -11745,12 +12480,15 @@
         <v>1</v>
       </c>
       <c r="N245" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O245" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="8" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B246" s="4" t="b">
         <v>0</v>
@@ -11789,12 +12527,15 @@
         <v>1</v>
       </c>
       <c r="N246" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O246" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="8" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B247" s="4" t="b">
         <v>0</v>
@@ -11833,12 +12574,15 @@
         <v>1</v>
       </c>
       <c r="N247" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O247" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="8" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B248" s="4" t="b">
         <v>0</v>
@@ -11877,12 +12621,15 @@
         <v>1</v>
       </c>
       <c r="N248" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O248" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="8" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B249" s="4" t="b">
         <v>0</v>
@@ -11921,12 +12668,15 @@
         <v>1</v>
       </c>
       <c r="N249" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O249" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="8" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B250" s="4" t="b">
         <v>0</v>
@@ -11965,12 +12715,15 @@
         <v>1</v>
       </c>
       <c r="N250" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O250" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="8" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B251" s="4" t="b">
         <v>0</v>
@@ -12009,12 +12762,15 @@
         <v>1</v>
       </c>
       <c r="N251" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O251" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="8" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B252" s="4" t="b">
         <v>0</v>
@@ -12053,12 +12809,15 @@
         <v>1</v>
       </c>
       <c r="N252" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O252" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="8" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B253" s="4" t="b">
         <v>0</v>
@@ -12097,12 +12856,15 @@
         <v>1</v>
       </c>
       <c r="N253" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O253" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="8" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B254" s="4" t="b">
         <v>0</v>
@@ -12141,12 +12903,15 @@
         <v>1</v>
       </c>
       <c r="N254" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O254" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="8" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B255" s="4" t="b">
         <v>0</v>
@@ -12185,12 +12950,15 @@
         <v>1</v>
       </c>
       <c r="N255" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O255" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="8" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B256" s="4" t="b">
         <v>0</v>
@@ -12229,12 +12997,15 @@
         <v>1</v>
       </c>
       <c r="N256" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O256" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="8" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B257" s="4" t="b">
         <v>0</v>
@@ -12273,12 +13044,15 @@
         <v>1</v>
       </c>
       <c r="N257" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O257" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="8" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B258" s="4" t="b">
         <v>0</v>
@@ -12317,12 +13091,15 @@
         <v>1</v>
       </c>
       <c r="N258" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O258" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="8" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B259" s="4" t="b">
         <v>0</v>
@@ -12361,12 +13138,15 @@
         <v>1</v>
       </c>
       <c r="N259" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O259" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="8" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B260" s="4" t="b">
         <v>0</v>
@@ -12405,12 +13185,15 @@
         <v>1</v>
       </c>
       <c r="N260" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O260" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="8" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B261" s="4" t="b">
         <v>0</v>
@@ -12449,12 +13232,15 @@
         <v>1</v>
       </c>
       <c r="N261" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O261" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="8" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B262" s="4" t="b">
         <v>0</v>
@@ -12493,12 +13279,15 @@
         <v>1</v>
       </c>
       <c r="N262" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O262" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B263" s="4" t="b">
         <v>0</v>
@@ -12537,12 +13326,15 @@
         <v>1</v>
       </c>
       <c r="N263" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O263" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="8" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B264" s="4" t="b">
         <v>0</v>
@@ -12581,6 +13373,9 @@
         <v>1</v>
       </c>
       <c r="N264" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O264" s="4" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>